<commit_message>
!!UWAGA!! Dodanie nowego pola w bazie danych!! <- dodano pole person w project, żeby moc gdzieś trzymać imię i nazwisko osoby kontaktowej - jest to w jednym polu. (Stosowne zmiany w requests.txt , models.py, schemas.py i dbFiller.py). + dodanie w tworzeniu z forms odczytu osoby
W main na endpoincie Student/Group/{id} w contact_info dodano pole person na tą informację

Aktualizacja Admin/Reservations żeby dawało id rezerwacji
</commit_message>
<xml_diff>
--- a/Backend/docs/KPZ_FORMS.xlsx
+++ b/Backend/docs/KPZ_FORMS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zakiashefa/Desktop/ProjektLaby/Kolos_JP/KPZ---New-webpage-/Backend/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\KPZ---New-webpage-\Backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A870088-6022-DA40-9932-65B0121AB412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF8EF1D-3863-48FE-9BAF-C53F55A56F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45280" yWindow="-15300" windowWidth="24280" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Liczba odpowiedzi 1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Sygnatura czasowa</t>
   </si>
@@ -114,13 +114,98 @@
   </si>
   <si>
     <t xml:space="preserve">siema </t>
+  </si>
+  <si>
+    <t>Comarch</t>
+  </si>
+  <si>
+    <t>Wszystkomat</t>
+  </si>
+  <si>
+    <t>Celem projektu jest opracowanie automatu paczkowego oraz systemu do dystrybucji paczek. Do realizacji przez grupę projektową jest część software i hardware.
+W części software do realizacji backend obsługujący system rozproszonych automatów paczkowych, frontend oraz aplikacja mobilna.
+W części hardware opracowanie przeskalowanego modelu automatu paczkowego z interfejsem dla użytkownika, systemu otwierającego skrytki, lokalne oraz zdalne sterowanie skrytkami.</t>
+  </si>
+  <si>
+    <t>Konsultacje merytoryczne ze strony pracownika firmy.</t>
+  </si>
+  <si>
+    <t>Comarch Comarchowski</t>
+  </si>
+  <si>
+    <t>Wersja Japońska:
+戦略的頭脳で知られる奈良シカマルは、隠された村・木ノ葉隠れの村で、古来より伝わる謎めいた囲碁のルールに出会う。しかし、ゲームの仮想世界は人工知能納豆によって脅かされ、プレイヤーたちを恐怖に陥れ始めた。
+シカマルは挑戦することを決意し、仲間とともに、最先端の人工知能納豆アルゴリズムをも欺くことができる古代のルールを探している。新たなルールを発見し、それを実行することで、秘策の里の平穏を取り戻そうというのだ。戦略家魂を持ち、シカマルの壮大な冒険を手助けしたい方は、ぜひご参加ください！一緒に、伝統と革新が融合した囲碁のプラットフォームを作り、戦略の世界に新たなフロンティアを発見しましょう！
+タスクの説明
+通常の囲碁ゲームでは、一定の大きさの碁盤（9路盤、13路盤、19路盤など）で対局する。囲碁プレイヤーにとって、周期的な碁盤で対局してみることは興味深い経験になるだろう。周期碁盤は一定の大きさ（例えば9x9）を持つが、境界はない。碁盤の代わりに、上下左右に同じ配置の牌を持つ別の碁盤があると想像することができる。このゲームでは、ズームインやズームアウトができるようにして、何が起こっているのかをよく見渡せるようにし、たとえば形を分析するときに、よりよい判断ができるようにする。
+野心的な人のために、球体（この場合、上辺と下辺だけが存在し、辺は存在しない）や立方体（角で盤面が崩れるのが面白く、追加のゲーム戦略を定義する必要がある）上にゲーム盤を作成するオプションもある。
+テクノロジー
+- フロントエンドのAngularまたはReact
+- 厳選されたグラフィックライブラリのサポート
+- UnityまたはUnreal Engine
+Wersja Polska:
+W Ukrytej Wiosce 木ノ葉隠れの村 Shikamaru Nara, znany ze swojego strategicznego umysłu, natrafił na tajemnicze starożytne zasady gry w Go, które obiecywały rewolucję w świecie strategii. Jednakże, wirtualny świat gry został zagrożony przez Sztuczną Inteligencję 納豆, która zaczęła terroryzować graczy.
+Shikamaru postanowił podjąć wyzwanie i wraz z przyjaciółmi poszukuje tych starożytnych zasad, zdolnych zwieść nawet najbardziej zaawansowane algorytmy A.I. 納豆. Wspólnie zamierzają odkryć i zaimplementować te nowe zasady, przywracając spokój 木ノ葉隠れの村. Jeśli masz duszę stratega i chcesz pomóc Shikamaru w tej epickiej przygodzie, dołącz do nas! Razem możemy stworzyć platformę do gry w Go, łącząc tradycję z innowacją, i odkryć nowe granice w świecie strategii!
+Opis zadania:
+W zwykłej grze w go gramy na planszy o określonym rozmiarze (np. 9x9, 13x13 lub 19x19). Ciekawym doświadczeniem dla graczy go byłoby spróbowanie gry na planszy cyklicznej. Cykliczna plansza ma określony rozmiar (np. 9x9), ale nie ma granic. Można to sobie wyobrazić tak, że zamiast planszy jest inna plansza z taką samą konfiguracją kamieni powyżej, poniżej, a także po lewej i prawej stronie. Gra powinna pozwalać na powiększanie i pomniejszanie, aby uzyskać dobrą perspektywę na to, co się dzieje, aby podejmować lepsze decyzje podczas np. analizowania kształtów.
+Dla ambitnych również opcja stworzenia planszy do gry na kuli (wtedy istnieje tylko krawędź górna i dolna, nie istnieją boczne) oraz na sześcianie (ciekawe załamanie planszy w rogach które wymaga określenia dodatkowych strategii gry)
+Technologia:
+- Frontend Angular lub React
+- Wsparcie wybranymi bibliotekami graficznymi
+- Dla chętnych Unity lub Unreal Engine</t>
+  </si>
+  <si>
+    <t>Delloite</t>
+  </si>
+  <si>
+    <t>Pracwonik Deloitte</t>
+  </si>
+  <si>
+    <t>Go no Jutsu: Shikamaru's Challenge</t>
+  </si>
+  <si>
+    <t>estigiti</t>
+  </si>
+  <si>
+    <t>Inteligentne przejście dla pieszych</t>
+  </si>
+  <si>
+    <t>Spaghetti Bolognese</t>
+  </si>
+  <si>
+    <t>Każdy z nas zna co najmniej jedno skrzyżowanie, na którym czas trwania zielonego światła przy przejściu dla pieszych zdaje się być lepiej dostosowany dla biegaczy niż dla przeciętnej osoby. Co jednak, kiedy osoba chcąca przejść przez ulicę ma większe potrzeby i wymaga wydłużenia czasu przejścia? Ten projekt ma na celu zbudowanie systemu, który za pomocą analizy strumienia wideo z kamery będzie w stanie odpowiednio dostosować czas sygnalizacji świetlnej do potrzeb przechodzących przez pasy osób starszych, z niepełnosprawnościami, rodziców z dziećmi, osób z bagażem czy grupy uczniów i jednocześnie zwiększyć ich bezpieczeństwo na drodze.</t>
+  </si>
+  <si>
+    <t>estigiti@example.com</t>
+  </si>
+  <si>
+    <t>delloite@example.com</t>
+  </si>
+  <si>
+    <t>fund@example.com</t>
+  </si>
+  <si>
+    <t>Rozwój Rozwojwoski</t>
+  </si>
+  <si>
+    <t>Fundacja wspierania innowacyjności badań i rozwoju</t>
+  </si>
+  <si>
+    <t>MedFolder</t>
+  </si>
+  <si>
+    <t>Celem projektu jest budowa systemu służącego do rejestracji, przechowywania, analizowania i łatwego przeglądania, w tym pełnotekstowego, wyników badań medycznych. Zakłada się, że dane będą mogły być wprowadzane poprzez: wgranie pliku; wykonanie zdjęcia (np. wydrukowanej kartki z wynikami laboratoryjnymi, bądź opisem innego rodzaju badań); wykonanie zdjęcia wyświetlacza medycznego urządzenia pomiarowego; pobranie danych z urządzeń posiadających stosowny interfejs; ręczne wprowadzenie danych; nagranie głosowe. Jednym z istotniejszych zagadnień jest dobór odpowiednich narzędzi do rozpoznawania obrazów, rozpoznawania tekstu i rozpoznawania mowy. Ważnym elementem aplikacji powinna być też możliwość wykonywania zestawień i raportów z zapisanych wyników badań. Preferowane technologie: Java / Spring, Python.</t>
+  </si>
+  <si>
+    <t>Konsultacje merytoryczne ze strony pracownika firmy.
+Nadzór merytoryczny pracownika firmy nad całością lub fragmentami projektu.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -161,6 +246,29 @@
       <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF471F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -185,13 +293,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -411,24 +530,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="18.83203125" customWidth="1"/>
+    <col min="1" max="6" width="18.77734375" customWidth="1"/>
     <col min="7" max="7" width="23.33203125" customWidth="1"/>
     <col min="8" max="10" width="26.6640625" customWidth="1"/>
-    <col min="11" max="11" width="28.5" customWidth="1"/>
+    <col min="11" max="11" width="28.44140625" customWidth="1"/>
     <col min="12" max="12" width="55.6640625" customWidth="1"/>
-    <col min="13" max="20" width="18.83203125" customWidth="1"/>
+    <col min="13" max="20" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +600,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>19</v>
       </c>
@@ -513,30 +632,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>123456789</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>17</v>
+      <c r="E3" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -545,30 +667,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D4">
-        <v>123456789</v>
+        <v>987654321</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -577,30 +702,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>123456789</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -609,21 +737,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6">
+        <v>765432198</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
       <c r="K6">
         <v>1</v>
       </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="7" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{50A2C93E-D7DA-724C-A75D-8528F5F4BF6C}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{B11CDEA2-854D-2849-A7F6-D3B403CD1138}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{2BDC0922-9BA5-EC4A-99B7-F037E2BA0F70}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{483A9348-7134-C44F-92AC-6B4FB182445C}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{BB5E7D38-AB69-4AA1-986D-5DB281B31193}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>